<commit_message>
consulta_cnpj_esalva_excel em massa 01/04/2025
</commit_message>
<xml_diff>
--- a/CNPJ.xlsx
+++ b/CNPJ.xlsx
@@ -455,7 +455,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="143" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -726,14 +726,11 @@
           <t>GOOGLE INTERNATIONAL LLC</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
       <c r="E6" t="inlineStr">
         <is>
           <t>1600 AMPHITHEATER PARKWAY</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>EXTERIOR</t>
@@ -744,7 +741,6 @@
           <t>EX</t>
         </is>
       </c>
-      <c r="I6" t="inlineStr"/>
       <c r="J6" t="inlineStr">
         <is>
           <t>Holdings de instituições não-financeiras</t>
@@ -798,6 +794,366 @@
         </is>
       </c>
       <c r="J7" t="inlineStr">
+        <is>
+          <t>Atividades de cobranças e informações cadastrais</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>33.157.312/0001-62</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>IFOOD BENEFICIOS E SERVICOS LTDA.</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>(11) 3634-3360</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>juridico@ifood.com.br</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>AV DOS AUTONOMISTAS 1496</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>VILA YARA</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>06.020-902</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>Emissão de vales-alimentação, vales-transporte e similares</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>06.947.283/0001-60</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>GOOGLE INTERNATIONAL LLC</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>1600 AMPHITHEATER PARKWAY</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>EXTERIOR</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>Holdings de instituições não-financeiras</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>33.157.312/0001-62</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>IFOOD BENEFICIOS E SERVICOS LTDA.</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>(11) 3634-3360</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>juridico@ifood.com.br</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>AV DOS AUTONOMISTAS 1496</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>VILA YARA</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>06.020-902</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>Emissão de vales-alimentação, vales-transporte e similares</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>06.947.283/0001-60</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>GOOGLE INTERNATIONAL LLC</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>1600 AMPHITHEATER PARKWAY</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>EXTERIOR</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Holdings de instituições não-financeiras</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>10.573.521/0001-91</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>MERCADO PAGO INSTITUICAO DE PAGAMENTO LTDA</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>(11) 2121-1212</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>naoresponder@mercadolivre.com</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>1 AV AVENIDA DAS NACOES UNIDAS, 3003</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BONFIM</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>06.233-903</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Atividades de cobranças e informações cadastrais</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>33.157.312/0001-62</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>IFOOD BENEFICIOS E SERVICOS LTDA.</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>(11) 3634-3360</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>juridico@ifood.com.br</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>AV DOS AUTONOMISTAS 1496</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>VILA YARA</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>06.020-902</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>Emissão de vales-alimentação, vales-transporte e similares</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>06.947.283/0001-60</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>GOOGLE INTERNATIONAL LLC</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>1600 AMPHITHEATER PARKWAY</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>EXTERIOR</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>EX</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>Holdings de instituições não-financeiras</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>10.573.521/0001-91</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>MERCADO PAGO INSTITUICAO DE PAGAMENTO LTDA</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>(11) 2121-1212</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>naoresponder@mercadolivre.com</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>1 AV AVENIDA DAS NACOES UNIDAS, 3003</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>BONFIM</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>OSASCO</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>SP</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>06.233-903</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>Atividades de cobranças e informações cadastrais</t>
         </is>

</xml_diff>